<commit_message>
Oppdaterte omkodingstabell med dagens fylkesnummer
SVN-revisjon: 4154
</commit_message>
<xml_diff>
--- a/felles/kodeboker/fylke-rhf.xlsx
+++ b/felles/kodeboker/fylke-rhf.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\kvalreg\felles\kodeboker\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="24915" windowHeight="16665"/>
+    <workbookView xWindow="480" yWindow="50" windowWidth="24920" windowHeight="16670"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -16,13 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
-  <si>
-    <t>fylke_kode</t>
-  </si>
-  <si>
-    <t>fylke_tekst</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>rhf_kode</t>
   </si>
@@ -103,12 +102,27 @@
   </si>
   <si>
     <t>(Svalbard)</t>
+  </si>
+  <si>
+    <t>Trøndelag</t>
+  </si>
+  <si>
+    <t>fylker_historisk</t>
+  </si>
+  <si>
+    <t>fylker_tekst</t>
+  </si>
+  <si>
+    <t>fylker_oppdatert</t>
+  </si>
+  <si>
+    <t>ltmv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -149,6 +163,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -197,7 +214,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -232,7 +249,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -441,369 +458,518 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
+      <c r="D2">
+        <v>18</v>
       </c>
       <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2">
         <v>111919</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>17</v>
       </c>
       <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3">
         <v>111919</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>16</v>
       </c>
       <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4">
         <v>111919</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>15</v>
       </c>
       <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5">
         <v>111919</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>14</v>
       </c>
       <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6">
         <v>111919</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
         <v>6</v>
       </c>
+      <c r="D7">
+        <v>13</v>
+      </c>
       <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7">
         <v>111919</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
         <v>12</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
       <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8">
         <v>111919</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>11</v>
       </c>
       <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9">
         <v>111919</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
       </c>
       <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10">
         <v>111919</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>9</v>
       </c>
       <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11">
         <v>111919</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+      <c r="E12">
         <v>2</v>
       </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12">
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12">
         <v>100021</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>7</v>
+      </c>
+      <c r="E13">
         <v>2</v>
       </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13">
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13">
         <v>100021</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C14">
+        <v>14</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
         <v>2</v>
       </c>
-      <c r="D14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14">
+      <c r="F14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14">
         <v>100021</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15">
         <v>3</v>
       </c>
-      <c r="D15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15">
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15">
         <v>100024</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C16">
+        <v>50</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
         <v>3</v>
       </c>
-      <c r="D16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16">
+      <c r="F16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16">
         <v>100024</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C17">
+        <v>50</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
         <v>3</v>
       </c>
-      <c r="D17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17">
+      <c r="F17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17">
         <v>100024</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>25</v>
+        <v>18</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
       </c>
       <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18">
         <v>100022</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C19">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
       </c>
       <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19">
         <v>100022</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C20">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
-        <v>25</v>
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
       </c>
       <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20">
         <v>100022</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C21">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
       </c>
       <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21">
         <v>100022</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>50</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22">
+        <v>50</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22">
+        <v>100024</v>
       </c>
     </row>
   </sheetData>
@@ -817,7 +983,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -829,7 +995,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fikset fylke-kodeboka til å ha en rekkefølge for LTMV
SVN-revisjon: 4276
</commit_message>
<xml_diff>
--- a/felles/kodeboker/fylke-rhf.xlsx
+++ b/felles/kodeboker/fylke-rhf.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="50" windowWidth="24920" windowHeight="16670"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="24915" windowHeight="16665"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
     <t>fylker_oppdatert</t>
   </si>
   <si>
-    <t>ltmv</t>
+    <t>fylker_ltmv</t>
   </si>
 </sst>
 </file>
@@ -461,12 +461,12 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -489,7 +489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -512,7 +512,7 @@
         <v>111919</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -535,7 +535,7 @@
         <v>111919</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -558,7 +558,7 @@
         <v>111919</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -581,7 +581,7 @@
         <v>111919</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -604,7 +604,7 @@
         <v>111919</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -627,7 +627,7 @@
         <v>111919</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -650,7 +650,7 @@
         <v>111919</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -673,7 +673,7 @@
         <v>111919</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -696,7 +696,7 @@
         <v>111919</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -719,7 +719,7 @@
         <v>111919</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -742,7 +742,7 @@
         <v>100021</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -765,7 +765,7 @@
         <v>100021</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
@@ -788,7 +788,7 @@
         <v>100021</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
@@ -811,7 +811,7 @@
         <v>100024</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
@@ -834,7 +834,7 @@
         <v>100024</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
@@ -857,7 +857,7 @@
         <v>100024</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
@@ -880,7 +880,7 @@
         <v>100022</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
@@ -903,7 +903,7 @@
         <v>100022</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
@@ -926,7 +926,7 @@
         <v>100022</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>21</v>
       </c>
@@ -949,7 +949,7 @@
         <v>100022</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>50</v>
       </c>
@@ -983,7 +983,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -995,7 +995,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Oppdatert filen med nyeste fylkesinndeling
SVN-revisjon: 5306
</commit_message>
<xml_diff>
--- a/felles/kodeboker/fylke-rhf.xlsx
+++ b/felles/kodeboker/fylke-rhf.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
   <si>
     <t>rhf_kode</t>
   </si>
@@ -117,6 +117,24 @@
   </si>
   <si>
     <t>fylker_ltmv</t>
+  </si>
+  <si>
+    <t>Viken</t>
+  </si>
+  <si>
+    <t>Innlandet</t>
+  </si>
+  <si>
+    <t>Vestfold og Telemark</t>
+  </si>
+  <si>
+    <t>Agder</t>
+  </si>
+  <si>
+    <t>Vestland</t>
+  </si>
+  <si>
+    <t>Troms og Finnmark</t>
   </si>
 </sst>
 </file>
@@ -458,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,10 +515,10 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="D2">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -520,10 +538,10 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D3">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -546,7 +564,7 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -566,10 +584,10 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="D5">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -589,10 +607,10 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="D6">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -612,10 +630,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D7">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -635,10 +653,10 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D8">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -658,10 +676,10 @@
         <v>11</v>
       </c>
       <c r="C9">
+        <v>38</v>
+      </c>
+      <c r="D9">
         <v>8</v>
-      </c>
-      <c r="D9">
-        <v>11</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -681,10 +699,10 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="D10">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -704,10 +722,10 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="D11">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -730,7 +748,7 @@
         <v>11</v>
       </c>
       <c r="D12">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -750,10 +768,10 @@
         <v>16</v>
       </c>
       <c r="C13">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="D13">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -773,10 +791,10 @@
         <v>17</v>
       </c>
       <c r="C14">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="D14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -799,7 +817,7 @@
         <v>15</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E15">
         <v>3</v>
@@ -822,7 +840,7 @@
         <v>50</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E16">
         <v>3</v>
@@ -845,7 +863,7 @@
         <v>50</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E17">
         <v>3</v>
@@ -868,7 +886,7 @@
         <v>18</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E18">
         <v>4</v>
@@ -888,10 +906,10 @@
         <v>24</v>
       </c>
       <c r="C19">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19">
         <v>4</v>
@@ -911,7 +929,7 @@
         <v>25</v>
       </c>
       <c r="C20">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -960,7 +978,7 @@
         <v>50</v>
       </c>
       <c r="D22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E22">
         <v>3</v>
@@ -970,6 +988,144 @@
       </c>
       <c r="G22">
         <v>100024</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23">
+        <v>30</v>
+      </c>
+      <c r="D23">
+        <v>11</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23">
+        <v>111919</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24">
+        <v>34</v>
+      </c>
+      <c r="D24">
+        <v>9</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24">
+        <v>111919</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>38</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25">
+        <v>38</v>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25">
+        <v>111919</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>42</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26">
+        <v>42</v>
+      </c>
+      <c r="D26">
+        <v>7</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26">
+        <v>111919</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27">
+        <v>46</v>
+      </c>
+      <c r="D27">
+        <v>5</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27">
+        <v>100021</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28">
+        <v>54</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28">
+        <v>100022</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Oppdatert koblingsfilen som innholder oversikt over gamle og nye fylker
SVN-revisjon: 6885
</commit_message>
<xml_diff>
--- a/felles/kodeboker/fylke-rhf.xlsx
+++ b/felles/kodeboker/fylke-rhf.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
   <si>
     <t>rhf_kode</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>Troms og Finnmark</t>
+  </si>
+  <si>
+    <t>Møreogromsdal</t>
+  </si>
+  <si>
+    <t>Sognogfjordane</t>
   </si>
 </sst>
 </file>
@@ -476,11 +482,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -808,39 +812,39 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15">
+        <v>46</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15">
-        <v>15</v>
-      </c>
-      <c r="D15">
-        <v>4</v>
-      </c>
-      <c r="E15">
-        <v>3</v>
-      </c>
-      <c r="F15" t="s">
-        <v>19</v>
-      </c>
       <c r="G15">
-        <v>100024</v>
+        <v>100021</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C16">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E16">
         <v>3</v>
@@ -854,16 +858,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C17">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E17">
         <v>3</v>
@@ -877,62 +881,62 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C18">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G18">
-        <v>100022</v>
+        <v>100024</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19">
+        <v>50</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19" t="s">
         <v>19</v>
       </c>
-      <c r="B19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19">
-        <v>54</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>4</v>
-      </c>
-      <c r="F19" t="s">
-        <v>23</v>
-      </c>
       <c r="G19">
-        <v>100022</v>
+        <v>100024</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C20">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20">
         <v>4</v>
@@ -946,13 +950,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C21">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -969,85 +973,85 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C22">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F22" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G22">
-        <v>100024</v>
+        <v>100022</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C23">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D23">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F23" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="G23">
-        <v>111919</v>
+        <v>100022</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C24">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="D24">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F24" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="G24">
-        <v>111919</v>
+        <v>100024</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C25">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D25">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1061,16 +1065,16 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C26">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D26">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -1084,47 +1088,93 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C27">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D27">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="G27">
-        <v>100021</v>
+        <v>111919</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
+        <v>42</v>
+      </c>
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28">
+        <v>42</v>
+      </c>
+      <c r="D28">
+        <v>7</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28">
+        <v>111919</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>46</v>
+      </c>
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29">
+        <v>46</v>
+      </c>
+      <c r="D29">
+        <v>5</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29">
+        <v>100021</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>54</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>37</v>
       </c>
-      <c r="C28">
+      <c r="C30">
         <v>54</v>
       </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28">
-        <v>4</v>
-      </c>
-      <c r="F28" t="s">
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+      <c r="F30" t="s">
         <v>23</v>
       </c>
-      <c r="G28">
+      <c r="G30">
         <v>100022</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fjernet en midlertidig tilpasning av kodebok-filen fylke-rhf.xlsx
SVN-revisjon: 6924
</commit_message>
<xml_diff>
--- a/felles/kodeboker/fylke-rhf.xlsx
+++ b/felles/kodeboker/fylke-rhf.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
   <si>
     <t>rhf_kode</t>
   </si>
@@ -135,12 +135,6 @@
   </si>
   <si>
     <t>Troms og Finnmark</t>
-  </si>
-  <si>
-    <t>Møreogromsdal</t>
-  </si>
-  <si>
-    <t>Sognogfjordane</t>
   </si>
 </sst>
 </file>
@@ -482,7 +476,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -812,39 +806,39 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="C15">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F15" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G15">
-        <v>100021</v>
+        <v>100024</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C16">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E16">
         <v>3</v>
@@ -858,16 +852,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C17">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E17">
         <v>3</v>
@@ -881,62 +875,62 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C18">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F18" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G18">
-        <v>100024</v>
+        <v>100022</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C19">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G19">
-        <v>100024</v>
+        <v>100022</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C20">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20">
         <v>4</v>
@@ -950,13 +944,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C21">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -973,85 +967,85 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C22">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G22">
-        <v>100022</v>
+        <v>100024</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C23">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E23">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="G23">
-        <v>100022</v>
+        <v>111919</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C24">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="D24">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="G24">
-        <v>100024</v>
+        <v>111919</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C25">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D25">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1065,16 +1059,16 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C26">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D26">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -1088,93 +1082,47 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C27">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D27">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="G27">
-        <v>111919</v>
+        <v>100021</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C28">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D28">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F28" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="G28">
-        <v>111919</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>46</v>
-      </c>
-      <c r="B29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29">
-        <v>46</v>
-      </c>
-      <c r="D29">
-        <v>5</v>
-      </c>
-      <c r="E29">
-        <v>2</v>
-      </c>
-      <c r="F29" t="s">
-        <v>15</v>
-      </c>
-      <c r="G29">
-        <v>100021</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>54</v>
-      </c>
-      <c r="B30" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30">
-        <v>54</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30">
-        <v>4</v>
-      </c>
-      <c r="F30" t="s">
-        <v>23</v>
-      </c>
-      <c r="G30">
         <v>100022</v>
       </c>
     </row>

</xml_diff>